<commit_message>
Add custom email feature
</commit_message>
<xml_diff>
--- a/demo/demo_subs.xlsx
+++ b/demo/demo_subs.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\Projects\mailing_list\demo\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{0B42072E-E84C-4975-92F2-4F4AB911FB29}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A41706D6-AD5B-49FF-A8F7-8DE6D175FBA7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-110" yWindow="-110" windowWidth="19420" windowHeight="10300" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -36,7 +36,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="10" uniqueCount="10">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="12" uniqueCount="12">
   <si>
     <t>test1@gmail.com</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>test10@gmail.com</t>
+  </si>
+  <si>
+    <t>test1</t>
+  </si>
+  <si>
+    <t>test2</t>
   </si>
 </sst>
 </file>
@@ -398,7 +404,7 @@
   <dimension ref="A1:D10"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="D9" sqref="D9"/>
+      <selection activeCell="B3" sqref="B3"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
@@ -410,11 +416,17 @@
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
+      <c r="B1" t="s">
+        <v>10</v>
+      </c>
       <c r="D1" s="2"/>
     </row>
     <row r="2" spans="1:4" x14ac:dyDescent="0.35">
       <c r="A2" s="1" t="s">
         <v>1</v>
+      </c>
+      <c r="B2" t="s">
+        <v>11</v>
       </c>
       <c r="D2" s="2"/>
     </row>

</xml_diff>